<commit_message>
Remove allocation tracking functionality
- Remove allocationPercentage field from ProjectAssignment schema
- Remove redundant code column from ProjectReport page
- Remove Total Allocation and Capacity Status from StaffDetail
- Remove allocation fields from all backend controllers and services
- Remove allocation from reports and Excel exports
- Clean up frontend types and UI components

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CM Asia_Staffing List - 2025.09.09_2.xlsx
+++ b/CM Asia_Staffing List - 2025.09.09_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\timlihk\staffing-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C020C1B-76D9-4533-9D84-F70C39B7B799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD770AC-496B-41C5-8D5E-E2EC1A718D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16605" yWindow="1650" windowWidth="31035" windowHeight="17145" xr2:uid="{EACFB4C6-21DB-44FC-A25C-B238E43844DC}"/>
+    <workbookView xWindow="20415" yWindow="3195" windowWidth="31035" windowHeight="17145" xr2:uid="{EACFB4C6-21DB-44FC-A25C-B238E43844DC}"/>
   </bookViews>
   <sheets>
     <sheet name="2. Staffing List by Project" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="258">
   <si>
     <t>Fortune</t>
   </si>
@@ -804,6 +804,15 @@
   </si>
   <si>
     <t>Project_name</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Hearing</t>
+  </si>
+  <si>
+    <t>Pre-A1</t>
   </si>
 </sst>
 </file>
@@ -1243,16 +1252,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08789A1-C03F-40A0-9C66-8858233A8AC1}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1372,7 +1381,9 @@
       <c r="N2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="8"/>
+      <c r="O2" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8" t="s">
         <v>214</v>
@@ -1417,7 +1428,9 @@
       <c r="N3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="8"/>
+      <c r="O3" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8" t="s">
         <v>215</v>
@@ -1462,7 +1475,9 @@
       <c r="N4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="8"/>
+      <c r="O4" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8" t="s">
         <v>191</v>
@@ -1506,7 +1521,9 @@
       <c r="N5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8" t="s">
         <v>163</v>
@@ -1552,6 +1569,9 @@
       <c r="N6" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="O6" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="Q6" s="8" t="s">
         <v>216</v>
       </c>
@@ -1589,6 +1609,9 @@
       </c>
       <c r="N7" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="Q7" s="8" t="s">
         <v>129</v>
@@ -1631,7 +1654,9 @@
       <c r="N8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="8"/>
+      <c r="O8" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8" t="s">
         <v>217</v>
@@ -1676,7 +1701,9 @@
       <c r="N9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="8"/>
+      <c r="O9" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8" t="s">
         <v>218</v>
@@ -1719,7 +1746,9 @@
       <c r="N10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="8"/>
+      <c r="O10" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8" t="s">
         <v>218</v>
@@ -1766,7 +1795,9 @@
       <c r="N11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="8"/>
+      <c r="O11" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="8" t="s">
         <v>219</v>
@@ -1811,7 +1842,9 @@
       <c r="N12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="8"/>
+      <c r="O12" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="8" t="s">
         <v>220</v>
@@ -1857,7 +1890,9 @@
       <c r="N13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="8"/>
+      <c r="O13" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="8" t="s">
         <v>192</v>
@@ -1906,7 +1941,9 @@
       <c r="N14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="8"/>
+      <c r="O14" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8" t="s">
         <v>193</v>
@@ -1951,6 +1988,9 @@
       </c>
       <c r="N15" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="Q15" s="8" t="s">
         <v>164</v>
@@ -2033,6 +2073,9 @@
       <c r="N17" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="O17" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="Q17" s="8" t="s">
         <v>162</v>
       </c>
@@ -2078,7 +2121,9 @@
       <c r="N18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="8"/>
+      <c r="O18" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="8" t="s">
         <v>162</v>
@@ -2121,7 +2166,9 @@
       <c r="N19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O19" s="8"/>
+      <c r="O19" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="8" t="s">
         <v>129</v>
@@ -2164,7 +2211,9 @@
       <c r="N20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="8"/>
+      <c r="O20" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="P20" s="8"/>
       <c r="Q20" s="8" t="s">
         <v>129</v>
@@ -2194,6 +2243,9 @@
       <c r="N21" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="O21" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q21" s="8" t="s">
         <v>178</v>
       </c>
@@ -2230,6 +2282,9 @@
       </c>
       <c r="N22" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="Q22" s="8" t="s">
         <v>167</v>
@@ -2317,7 +2372,9 @@
       <c r="N24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O24" s="8"/>
+      <c r="O24" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="8" t="s">
         <v>165</v>
@@ -2360,7 +2417,9 @@
       <c r="N25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O25" s="8"/>
+      <c r="O25" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="8" t="s">
         <v>166</v>
@@ -2405,7 +2464,9 @@
       <c r="N26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O26" s="8"/>
+      <c r="O26" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="8" t="s">
         <v>167</v>
@@ -2446,7 +2507,9 @@
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8" t="s">
         <v>165</v>
@@ -2491,7 +2554,9 @@
       <c r="N28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O28" s="8"/>
+      <c r="O28" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8" t="s">
         <v>167</v>
@@ -2538,7 +2603,9 @@
       <c r="N29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O29" s="8"/>
+      <c r="O29" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8" t="s">
         <v>168</v>
@@ -2581,7 +2648,9 @@
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="O30" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8" t="s">
         <v>169</v>
@@ -2626,6 +2695,9 @@
       <c r="N31" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="O31" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q31" s="8" t="s">
         <v>169</v>
       </c>
@@ -2668,6 +2740,9 @@
       <c r="N32" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="O32" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q32" s="8" t="s">
         <v>170</v>
       </c>
@@ -2710,6 +2785,9 @@
       <c r="N33" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="O33" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q33" s="8" t="s">
         <v>167</v>
       </c>
@@ -2752,6 +2830,9 @@
       <c r="N34" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="O34" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q34" s="8" t="s">
         <v>167</v>
       </c>
@@ -2791,6 +2872,9 @@
       <c r="N35" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="O35" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q35" s="8" t="s">
         <v>167</v>
       </c>
@@ -2872,6 +2956,9 @@
       </c>
       <c r="N37" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="Q37" s="8" t="s">
         <v>167</v>
@@ -2993,6 +3080,9 @@
       <c r="N41" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="O41" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q41" s="8" t="s">
         <v>167</v>
       </c>
@@ -3055,6 +3145,9 @@
       <c r="N43" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="O43" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q43" s="8" t="s">
         <v>198</v>
       </c>
@@ -3094,6 +3187,9 @@
       </c>
       <c r="N44" s="8" t="s">
         <v>40</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="Q44" s="8" t="s">
         <v>201</v>
@@ -3152,6 +3248,9 @@
       <c r="N46" s="8" t="s">
         <v>207</v>
       </c>
+      <c r="O46" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q46" s="8" t="s">
         <v>169</v>
       </c>
@@ -3190,6 +3289,9 @@
       </c>
       <c r="N47" s="8" t="s">
         <v>204</v>
+      </c>
+      <c r="O47" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="Q47" s="8" t="s">
         <v>205</v>
@@ -3318,6 +3420,9 @@
       <c r="N51" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="O51" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="Q51" s="8" t="s">
         <v>210</v>
       </c>
@@ -3356,6 +3461,9 @@
       </c>
       <c r="N52" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="Q52" s="8" t="s">
         <v>170</v>
@@ -3443,7 +3551,9 @@
       <c r="N54" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O54" s="8"/>
+      <c r="O54" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="P54" s="8"/>
       <c r="Q54" s="8" t="s">
         <v>178</v>
@@ -3573,7 +3683,7 @@
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -3596,7 +3706,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -3625,7 +3735,7 @@
       <c r="P59" s="8"/>
       <c r="Q59" s="8"/>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -3654,7 +3764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -3677,7 +3787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -3700,7 +3810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>234</v>
       </c>
@@ -3717,7 +3827,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>235</v>
       </c>
@@ -3731,7 +3841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>39</v>
       </c>
@@ -3751,7 +3861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>41</v>
       </c>
@@ -3771,7 +3881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>43</v>
       </c>
@@ -3791,7 +3901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
@@ -3811,7 +3921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>46</v>
       </c>
@@ -3831,7 +3941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>47</v>
       </c>
@@ -3854,7 +3964,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>48</v>
       </c>
@@ -3877,7 +3987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:17" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>49</v>
       </c>
@@ -3902,7 +4012,7 @@
       <c r="P72"/>
       <c r="Q72"/>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>51</v>
       </c>
@@ -3929,7 +4039,7 @@
       <c r="P73" s="8"/>
       <c r="Q73" s="8"/>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>52</v>
       </c>
@@ -3949,7 +4059,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>54</v>
       </c>
@@ -3969,7 +4079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>56</v>
       </c>
@@ -3989,7 +4099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>57</v>
       </c>
@@ -4010,7 +4120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>58</v>
       </c>
@@ -4031,7 +4141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>59</v>
       </c>
@@ -4054,7 +4164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
@@ -4074,7 +4184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>62</v>
       </c>
@@ -4091,7 +4201,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -4111,7 +4221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>123</v>
       </c>
@@ -4134,7 +4244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>124</v>
       </c>
@@ -4154,7 +4264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -4174,7 +4284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -4194,7 +4304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>67</v>
       </c>
@@ -4208,7 +4318,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>68</v>
       </c>
@@ -4222,7 +4332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>84</v>
       </c>
@@ -4236,7 +4346,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -4256,7 +4366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>100</v>
       </c>
@@ -4273,7 +4383,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>116</v>
       </c>
@@ -4291,13 +4401,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q92" xr:uid="{F08789A1-C03F-40A0-9C66-8858233A8AC1}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="HK Trx"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q92" xr:uid="{F08789A1-C03F-40A0-9C66-8858233A8AC1}"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="70" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>